<commit_message>
epic! it works for a good file. now what about bad files and dates.
</commit_message>
<xml_diff>
--- a/src/freshStart/7.27.xlsx
+++ b/src/freshStart/7.27.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="18885" windowHeight="11160" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="9960" windowHeight="11295" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1597,8 +1597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O194"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1612,10 +1612,11 @@
     <col min="8" max="8" width="17.5703125" customWidth="1"/>
     <col min="9" max="9" width="7.42578125" customWidth="1"/>
     <col min="10" max="10" width="10" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" customWidth="1"/>
-    <col min="12" max="12" width="10" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" customWidth="1"/>
-    <col min="14" max="15" width="10" customWidth="1"/>
+    <col min="11" max="11" width="2.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" customWidth="1"/>
+    <col min="13" max="13" width="29.42578125" customWidth="1"/>
+    <col min="14" max="14" width="5.28515625" customWidth="1"/>
+    <col min="15" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">

</xml_diff>